<commit_message>
Eugenie  and removed password
</commit_message>
<xml_diff>
--- a/src/assets/Excells/CotisationSpeciale1.xlsx
+++ b/src/assets/Excells/CotisationSpeciale1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwamutalamiantezila/Documents/LukalaPhoto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6147BEA-BB48-9443-8240-F380B1FEA722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34772B2-A4BF-2F47-8786-8E5DF1E2CD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16240" xr2:uid="{68E375EF-7E04-A04A-8B5D-972BEA3F72AD}"/>
   </bookViews>
@@ -697,7 +697,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,11 +744,11 @@
         <v>10</v>
       </c>
       <c r="E2" s="13">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F2" s="13">
         <f>SUM(D2,E2)</f>
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -891,11 +891,11 @@
       </c>
       <c r="E9" s="16">
         <f>SUM(E2:E8)</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F9" s="17">
         <f>SUM(F2:F8)</f>
-        <v>170</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>